<commit_message>
Update freshwater catch data notes
</commit_message>
<xml_diff>
--- a/data-raw/freshwater-catch.xlsx
+++ b/data-raw/freshwater-catch.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\skrunchy2025\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74DE55E9-4C85-4643-9888-C6949CB1692C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFB62E85-4C26-4001-8636-1A5E3CC34E41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E0CDEE87-6CC2-4107-81B9-F1AD4EA649A7}"/>
   </bookViews>
@@ -86,13 +86,7 @@
     <t>1000 above / 2500 below from average 2010-2017 and old Elmer Fast data</t>
   </si>
   <si>
-    <t>RGS before 1995 may include Tyee - check</t>
-  </si>
-  <si>
     <t>2007, 2012 flood or persistent high water years</t>
-  </si>
-  <si>
-    <t>Total Skeena sport catch 1979 to 1996 separated into 2/3 catch below Terrace and 1/3 catch above Terrace (comment from E. Fast in '89)</t>
   </si>
   <si>
     <t>2011 high snow pack and low catches, flood early then avg flows</t>
@@ -123,6 +117,12 @@
   </si>
   <si>
     <t>FW Sport releases below Terrace</t>
+  </si>
+  <si>
+    <t>Total Skeena sport catch 1979 to 1996 separated into 2/3 catch below Terrace and 1/3 catch above Terrace (comment from E. Fast in 1989)</t>
+  </si>
+  <si>
+    <t>Notes</t>
   </si>
 </sst>
 </file>
@@ -276,9 +276,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -314,6 +311,7 @@
     <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -632,11 +630,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35E3952C-60AA-4AE7-A274-2D9A331D3C7B}">
-  <dimension ref="A1:BI185"/>
+  <dimension ref="A1:BI186"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O43" sqref="O43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -645,7 +643,7 @@
     <col min="2" max="3" width="8.7109375" style="1"/>
     <col min="4" max="4" width="7.140625" style="1" customWidth="1"/>
     <col min="5" max="12" width="8.7109375" style="1"/>
-    <col min="13" max="13" width="8.42578125" style="20" customWidth="1"/>
+    <col min="13" max="13" width="8.42578125" style="19" customWidth="1"/>
     <col min="14" max="22" width="7.5703125" style="1" customWidth="1"/>
     <col min="23" max="24" width="8.85546875" style="1" customWidth="1"/>
     <col min="25" max="28" width="7.5703125" style="1" customWidth="1"/>
@@ -671,7 +669,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:61" s="4" customFormat="1" ht="72" x14ac:dyDescent="0.2">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -680,16 +678,16 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="26" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="27" t="s">
+      <c r="G1" s="26" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
@@ -704,58 +702,58 @@
       <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="28" t="s">
-        <v>27</v>
-      </c>
-      <c r="M1" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="N1" s="27" t="s">
+      <c r="L1" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="27" t="s">
+      <c r="O1" s="26" t="s">
         <v>12</v>
       </c>
       <c r="P1" s="2"/>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="19"/>
-      <c r="S1" s="19"/>
-      <c r="T1" s="21"/>
-      <c r="U1" s="19"/>
-      <c r="V1" s="21"/>
-      <c r="W1" s="19"/>
-      <c r="X1" s="21"/>
-      <c r="Y1" s="19"/>
-      <c r="Z1" s="19"/>
-      <c r="AA1" s="19"/>
-      <c r="AB1" s="19"/>
-      <c r="AC1" s="19"/>
-      <c r="AD1" s="19"/>
-      <c r="AE1" s="19"/>
-      <c r="AF1" s="19"/>
-      <c r="AG1" s="19"/>
-      <c r="AH1" s="19"/>
-      <c r="AI1" s="19"/>
-      <c r="AJ1" s="19"/>
-      <c r="AK1" s="19"/>
-      <c r="AL1" s="19"/>
-      <c r="AM1" s="19"/>
-      <c r="AN1" s="19"/>
-      <c r="AO1" s="19"/>
-      <c r="AP1" s="19"/>
-      <c r="AQ1" s="19"/>
-      <c r="AR1" s="22"/>
-      <c r="AS1" s="22"/>
-      <c r="AT1" s="22"/>
-      <c r="AU1" s="22"/>
-      <c r="AV1" s="22"/>
-      <c r="AW1" s="22"/>
-      <c r="AX1" s="22"/>
-      <c r="AY1" s="22"/>
-      <c r="AZ1" s="22"/>
-      <c r="BA1" s="20"/>
-      <c r="BB1" s="20"/>
-      <c r="BC1" s="20"/>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="18"/>
+      <c r="S1" s="18"/>
+      <c r="T1" s="20"/>
+      <c r="U1" s="18"/>
+      <c r="V1" s="20"/>
+      <c r="W1" s="18"/>
+      <c r="X1" s="20"/>
+      <c r="Y1" s="18"/>
+      <c r="Z1" s="18"/>
+      <c r="AA1" s="18"/>
+      <c r="AB1" s="18"/>
+      <c r="AC1" s="18"/>
+      <c r="AD1" s="18"/>
+      <c r="AE1" s="18"/>
+      <c r="AF1" s="18"/>
+      <c r="AG1" s="18"/>
+      <c r="AH1" s="18"/>
+      <c r="AI1" s="18"/>
+      <c r="AJ1" s="18"/>
+      <c r="AK1" s="18"/>
+      <c r="AL1" s="18"/>
+      <c r="AM1" s="18"/>
+      <c r="AN1" s="18"/>
+      <c r="AO1" s="18"/>
+      <c r="AP1" s="18"/>
+      <c r="AQ1" s="18"/>
+      <c r="AR1" s="21"/>
+      <c r="AS1" s="21"/>
+      <c r="AT1" s="21"/>
+      <c r="AU1" s="21"/>
+      <c r="AV1" s="21"/>
+      <c r="AW1" s="21"/>
+      <c r="AX1" s="21"/>
+      <c r="AY1" s="21"/>
+      <c r="AZ1" s="21"/>
+      <c r="BA1" s="19"/>
+      <c r="BB1" s="19"/>
+      <c r="BC1" s="19"/>
       <c r="BD1" s="1"/>
     </row>
     <row r="2" spans="1:61" x14ac:dyDescent="0.2">
@@ -776,11 +774,11 @@
         <v>1410</v>
       </c>
       <c r="F2" s="6">
-        <f>ROUND((E2*2/3),0)</f>
+        <f t="shared" ref="F2:F19" si="1">ROUND((E2*2/3),0)</f>
         <v>940</v>
       </c>
       <c r="G2" s="6">
-        <f>E2-F2</f>
+        <f t="shared" ref="G2:G24" si="2">E2-F2</f>
         <v>470</v>
       </c>
       <c r="H2" s="7"/>
@@ -791,7 +789,7 @@
         <f>SUM(F2,H2,I2)</f>
         <v>940</v>
       </c>
-      <c r="M2" s="24">
+      <c r="M2" s="23">
         <f>SUM(J2,K2)</f>
         <v>0</v>
       </c>
@@ -852,19 +850,19 @@
         <v>3625</v>
       </c>
       <c r="F3" s="6">
-        <f>ROUND((E3*2/3),0)</f>
+        <f t="shared" si="1"/>
         <v>2417</v>
       </c>
       <c r="G3" s="6">
-        <f>E3-F3</f>
+        <f t="shared" si="2"/>
         <v>1208</v>
       </c>
       <c r="L3" s="7">
-        <f t="shared" ref="L3:L43" si="1">SUM(F3,H3,I3)</f>
+        <f t="shared" ref="L3:L43" si="3">SUM(F3,H3,I3)</f>
         <v>2417</v>
       </c>
-      <c r="M3" s="24">
-        <f t="shared" ref="M3:M43" si="2">SUM(J3,K3)</f>
+      <c r="M3" s="23">
+        <f t="shared" ref="M3:M43" si="4">SUM(J3,K3)</f>
         <v>0</v>
       </c>
       <c r="N3" s="1">
@@ -924,19 +922,19 @@
         <v>2210</v>
       </c>
       <c r="F4" s="6">
-        <f>ROUND((E4*2/3),0)</f>
-        <v>1473</v>
-      </c>
-      <c r="G4" s="6">
-        <f>E4-F4</f>
-        <v>737</v>
-      </c>
-      <c r="L4" s="7">
         <f t="shared" si="1"/>
         <v>1473</v>
       </c>
-      <c r="M4" s="24">
+      <c r="G4" s="6">
         <f t="shared" si="2"/>
+        <v>737</v>
+      </c>
+      <c r="L4" s="7">
+        <f t="shared" si="3"/>
+        <v>1473</v>
+      </c>
+      <c r="M4" s="23">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N4" s="1">
@@ -996,19 +994,19 @@
         <v>2230</v>
       </c>
       <c r="F5" s="6">
-        <f>ROUND((E5*2/3),0)</f>
-        <v>1487</v>
-      </c>
-      <c r="G5" s="6">
-        <f>E5-F5</f>
-        <v>743</v>
-      </c>
-      <c r="L5" s="7">
         <f t="shared" si="1"/>
         <v>1487</v>
       </c>
-      <c r="M5" s="24">
+      <c r="G5" s="6">
         <f t="shared" si="2"/>
+        <v>743</v>
+      </c>
+      <c r="L5" s="7">
+        <f t="shared" si="3"/>
+        <v>1487</v>
+      </c>
+      <c r="M5" s="23">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N5" s="1">
@@ -1068,19 +1066,19 @@
         <v>4366</v>
       </c>
       <c r="F6" s="6">
-        <f>ROUND((E6*2/3),0)</f>
-        <v>2911</v>
-      </c>
-      <c r="G6" s="6">
-        <f>E6-F6</f>
-        <v>1455</v>
-      </c>
-      <c r="L6" s="7">
         <f t="shared" si="1"/>
         <v>2911</v>
       </c>
-      <c r="M6" s="24">
+      <c r="G6" s="6">
         <f t="shared" si="2"/>
+        <v>1455</v>
+      </c>
+      <c r="L6" s="7">
+        <f t="shared" si="3"/>
+        <v>2911</v>
+      </c>
+      <c r="M6" s="23">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N6" s="1">
@@ -1123,78 +1121,78 @@
       <c r="BD6" s="7"/>
       <c r="BI6" s="7"/>
     </row>
-    <row r="7" spans="1:61" s="29" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="29">
+    <row r="7" spans="1:61" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="28">
         <v>1984</v>
       </c>
-      <c r="B7" s="29">
+      <c r="B7" s="28">
         <v>587</v>
       </c>
-      <c r="C7" s="29">
+      <c r="C7" s="28">
         <v>153</v>
       </c>
-      <c r="D7" s="29">
+      <c r="D7" s="28">
         <f t="shared" si="0"/>
         <v>740</v>
       </c>
-      <c r="E7" s="30">
+      <c r="E7" s="29">
         <v>2976</v>
       </c>
-      <c r="F7" s="30">
-        <f>ROUND((E7*2/3),0)</f>
-        <v>1984</v>
-      </c>
-      <c r="G7" s="30">
-        <f>E7-F7</f>
-        <v>992</v>
-      </c>
-      <c r="L7" s="31">
+      <c r="F7" s="29">
         <f t="shared" si="1"/>
         <v>1984</v>
       </c>
-      <c r="M7" s="32">
+      <c r="G7" s="29">
         <f t="shared" si="2"/>
+        <v>992</v>
+      </c>
+      <c r="L7" s="30">
+        <f t="shared" si="3"/>
+        <v>1984</v>
+      </c>
+      <c r="M7" s="31">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="N7" s="29">
+      <c r="N7" s="28">
         <v>1568</v>
       </c>
-      <c r="O7" s="31">
+      <c r="O7" s="30">
         <v>7900</v>
       </c>
-      <c r="P7" s="33"/>
-      <c r="Q7" s="33"/>
-      <c r="R7" s="33"/>
-      <c r="S7" s="33"/>
-      <c r="T7" s="31"/>
-      <c r="U7" s="31"/>
-      <c r="V7" s="31"/>
-      <c r="W7" s="31"/>
-      <c r="X7" s="31"/>
-      <c r="Y7" s="34"/>
-      <c r="Z7" s="34"/>
-      <c r="AA7" s="34"/>
-      <c r="AB7" s="34"/>
-      <c r="AC7" s="34"/>
-      <c r="AD7" s="31"/>
-      <c r="AE7" s="31"/>
-      <c r="AF7" s="31"/>
-      <c r="AG7" s="31"/>
-      <c r="AH7" s="31"/>
-      <c r="AI7" s="31"/>
-      <c r="AJ7" s="35"/>
-      <c r="AL7" s="31"/>
-      <c r="AM7" s="31"/>
-      <c r="AN7" s="31"/>
-      <c r="AO7" s="31"/>
-      <c r="AP7" s="31"/>
-      <c r="AQ7" s="31"/>
-      <c r="AS7" s="31"/>
-      <c r="AU7" s="31"/>
-      <c r="AW7" s="31"/>
-      <c r="AY7" s="31"/>
-      <c r="BD7" s="31"/>
-      <c r="BI7" s="31"/>
+      <c r="P7" s="32"/>
+      <c r="Q7" s="32"/>
+      <c r="R7" s="32"/>
+      <c r="S7" s="32"/>
+      <c r="T7" s="30"/>
+      <c r="U7" s="30"/>
+      <c r="V7" s="30"/>
+      <c r="W7" s="30"/>
+      <c r="X7" s="30"/>
+      <c r="Y7" s="33"/>
+      <c r="Z7" s="33"/>
+      <c r="AA7" s="33"/>
+      <c r="AB7" s="33"/>
+      <c r="AC7" s="33"/>
+      <c r="AD7" s="30"/>
+      <c r="AE7" s="30"/>
+      <c r="AF7" s="30"/>
+      <c r="AG7" s="30"/>
+      <c r="AH7" s="30"/>
+      <c r="AI7" s="30"/>
+      <c r="AJ7" s="34"/>
+      <c r="AL7" s="30"/>
+      <c r="AM7" s="30"/>
+      <c r="AN7" s="30"/>
+      <c r="AO7" s="30"/>
+      <c r="AP7" s="30"/>
+      <c r="AQ7" s="30"/>
+      <c r="AS7" s="30"/>
+      <c r="AU7" s="30"/>
+      <c r="AW7" s="30"/>
+      <c r="AY7" s="30"/>
+      <c r="BD7" s="30"/>
+      <c r="BI7" s="30"/>
     </row>
     <row r="8" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
@@ -1214,19 +1212,19 @@
         <v>2025</v>
       </c>
       <c r="F8" s="6">
-        <f>ROUND((E8*2/3),0)</f>
-        <v>1350</v>
-      </c>
-      <c r="G8" s="6">
-        <f>E8-F8</f>
-        <v>675</v>
-      </c>
-      <c r="L8" s="7">
         <f t="shared" si="1"/>
         <v>1350</v>
       </c>
-      <c r="M8" s="24">
+      <c r="G8" s="6">
         <f t="shared" si="2"/>
+        <v>675</v>
+      </c>
+      <c r="L8" s="7">
+        <f t="shared" si="3"/>
+        <v>1350</v>
+      </c>
+      <c r="M8" s="23">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N8" s="1">
@@ -1287,19 +1285,19 @@
         <v>3010</v>
       </c>
       <c r="F9" s="6">
-        <f>ROUND((E9*2/3),0)</f>
-        <v>2007</v>
-      </c>
-      <c r="G9" s="6">
-        <f>E9-F9</f>
-        <v>1003</v>
-      </c>
-      <c r="L9" s="7">
         <f t="shared" si="1"/>
         <v>2007</v>
       </c>
-      <c r="M9" s="24">
+      <c r="G9" s="6">
         <f t="shared" si="2"/>
+        <v>1003</v>
+      </c>
+      <c r="L9" s="7">
+        <f t="shared" si="3"/>
+        <v>2007</v>
+      </c>
+      <c r="M9" s="23">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N9" s="1">
@@ -1360,19 +1358,19 @@
         <v>2525</v>
       </c>
       <c r="F10" s="6">
-        <f>ROUND((E10*2/3),0)</f>
-        <v>1683</v>
-      </c>
-      <c r="G10" s="6">
-        <f>E10-F10</f>
-        <v>842</v>
-      </c>
-      <c r="L10" s="7">
         <f t="shared" si="1"/>
         <v>1683</v>
       </c>
-      <c r="M10" s="24">
+      <c r="G10" s="6">
         <f t="shared" si="2"/>
+        <v>842</v>
+      </c>
+      <c r="L10" s="7">
+        <f t="shared" si="3"/>
+        <v>1683</v>
+      </c>
+      <c r="M10" s="23">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N10" s="1">
@@ -1433,19 +1431,19 @@
         <v>3295</v>
       </c>
       <c r="F11" s="6">
-        <f>ROUND((E11*2/3),0)</f>
-        <v>2197</v>
-      </c>
-      <c r="G11" s="6">
-        <f>E11-F11</f>
-        <v>1098</v>
-      </c>
-      <c r="L11" s="7">
         <f t="shared" si="1"/>
         <v>2197</v>
       </c>
-      <c r="M11" s="24">
+      <c r="G11" s="6">
         <f t="shared" si="2"/>
+        <v>1098</v>
+      </c>
+      <c r="L11" s="7">
+        <f t="shared" si="3"/>
+        <v>2197</v>
+      </c>
+      <c r="M11" s="23">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N11" s="1">
@@ -1506,19 +1504,19 @@
         <v>4521</v>
       </c>
       <c r="F12" s="6">
-        <f>ROUND((E12*2/3),0)</f>
-        <v>3014</v>
-      </c>
-      <c r="G12" s="6">
-        <f>E12-F12</f>
-        <v>1507</v>
-      </c>
-      <c r="L12" s="7">
         <f t="shared" si="1"/>
         <v>3014</v>
       </c>
-      <c r="M12" s="24">
+      <c r="G12" s="6">
         <f t="shared" si="2"/>
+        <v>1507</v>
+      </c>
+      <c r="L12" s="7">
+        <f t="shared" si="3"/>
+        <v>3014</v>
+      </c>
+      <c r="M12" s="23">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N12" s="1">
@@ -1579,19 +1577,19 @@
         <v>3660</v>
       </c>
       <c r="F13" s="6">
-        <f>ROUND((E13*2/3),0)</f>
-        <v>2440</v>
-      </c>
-      <c r="G13" s="6">
-        <f>E13-F13</f>
-        <v>1220</v>
-      </c>
-      <c r="L13" s="7">
         <f t="shared" si="1"/>
         <v>2440</v>
       </c>
-      <c r="M13" s="24">
+      <c r="G13" s="6">
         <f t="shared" si="2"/>
+        <v>1220</v>
+      </c>
+      <c r="L13" s="7">
+        <f t="shared" si="3"/>
+        <v>2440</v>
+      </c>
+      <c r="M13" s="23">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N13" s="1">
@@ -1652,19 +1650,19 @@
         <v>4440</v>
       </c>
       <c r="F14" s="6">
-        <f>ROUND((E14*2/3),0)</f>
-        <v>2960</v>
-      </c>
-      <c r="G14" s="6">
-        <f>E14-F14</f>
-        <v>1480</v>
-      </c>
-      <c r="L14" s="7">
         <f t="shared" si="1"/>
         <v>2960</v>
       </c>
-      <c r="M14" s="24">
+      <c r="G14" s="6">
         <f t="shared" si="2"/>
+        <v>1480</v>
+      </c>
+      <c r="L14" s="7">
+        <f t="shared" si="3"/>
+        <v>2960</v>
+      </c>
+      <c r="M14" s="23">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N14" s="1">
@@ -1725,19 +1723,19 @@
         <v>5030</v>
       </c>
       <c r="F15" s="6">
-        <f>ROUND((E15*2/3),0)</f>
-        <v>3353</v>
-      </c>
-      <c r="G15" s="6">
-        <f>E15-F15</f>
-        <v>1677</v>
-      </c>
-      <c r="L15" s="7">
         <f t="shared" si="1"/>
         <v>3353</v>
       </c>
-      <c r="M15" s="24">
+      <c r="G15" s="6">
         <f t="shared" si="2"/>
+        <v>1677</v>
+      </c>
+      <c r="L15" s="7">
+        <f t="shared" si="3"/>
+        <v>3353</v>
+      </c>
+      <c r="M15" s="23">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N15" s="1">
@@ -1798,19 +1796,19 @@
         <v>6832</v>
       </c>
       <c r="F16" s="6">
-        <f>ROUND((E16*2/3),0)</f>
-        <v>4555</v>
-      </c>
-      <c r="G16" s="6">
-        <f>E16-F16</f>
-        <v>2277</v>
-      </c>
-      <c r="L16" s="7">
         <f t="shared" si="1"/>
         <v>4555</v>
       </c>
-      <c r="M16" s="24">
+      <c r="G16" s="6">
         <f t="shared" si="2"/>
+        <v>2277</v>
+      </c>
+      <c r="L16" s="7">
+        <f t="shared" si="3"/>
+        <v>4555</v>
+      </c>
+      <c r="M16" s="23">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N16" s="1">
@@ -1871,19 +1869,19 @@
         <v>2200</v>
       </c>
       <c r="F17" s="6">
-        <f>ROUND((E17*2/3),0)</f>
-        <v>1467</v>
-      </c>
-      <c r="G17" s="6">
-        <f>E17-F17</f>
-        <v>733</v>
-      </c>
-      <c r="L17" s="7">
         <f t="shared" si="1"/>
         <v>1467</v>
       </c>
-      <c r="M17" s="24">
+      <c r="G17" s="6">
         <f t="shared" si="2"/>
+        <v>733</v>
+      </c>
+      <c r="L17" s="7">
+        <f t="shared" si="3"/>
+        <v>1467</v>
+      </c>
+      <c r="M17" s="23">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N17" s="1">
@@ -1944,19 +1942,19 @@
         <v>2798</v>
       </c>
       <c r="F18" s="6">
-        <f>ROUND((E18*2/3),0)</f>
-        <v>1865</v>
-      </c>
-      <c r="G18" s="6">
-        <f>E18-F18</f>
-        <v>933</v>
-      </c>
-      <c r="L18" s="7">
         <f t="shared" si="1"/>
         <v>1865</v>
       </c>
-      <c r="M18" s="24">
+      <c r="G18" s="6">
         <f t="shared" si="2"/>
+        <v>933</v>
+      </c>
+      <c r="L18" s="7">
+        <f t="shared" si="3"/>
+        <v>1865</v>
+      </c>
+      <c r="M18" s="23">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N18" s="1">
@@ -2017,19 +2015,19 @@
         <v>1250</v>
       </c>
       <c r="F19" s="6">
-        <f>ROUND((E19*2/3),0)</f>
-        <v>833</v>
-      </c>
-      <c r="G19" s="6">
-        <f>E19-F19</f>
-        <v>417</v>
-      </c>
-      <c r="L19" s="7">
         <f t="shared" si="1"/>
         <v>833</v>
       </c>
-      <c r="M19" s="24">
+      <c r="G19" s="6">
         <f t="shared" si="2"/>
+        <v>417</v>
+      </c>
+      <c r="L19" s="7">
+        <f t="shared" si="3"/>
+        <v>833</v>
+      </c>
+      <c r="M19" s="23">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N19" s="1">
@@ -2093,15 +2091,15 @@
         <v>2500</v>
       </c>
       <c r="G20" s="11">
-        <f>E20-F20</f>
+        <f t="shared" si="2"/>
         <v>1000</v>
       </c>
       <c r="L20" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2500</v>
       </c>
-      <c r="M20" s="24">
-        <f t="shared" si="2"/>
+      <c r="M20" s="23">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N20" s="1">
@@ -2164,15 +2162,15 @@
         <v>2500</v>
       </c>
       <c r="G21" s="11">
-        <f>E21-F21</f>
+        <f t="shared" si="2"/>
         <v>1000</v>
       </c>
       <c r="L21" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2500</v>
       </c>
-      <c r="M21" s="24">
-        <f t="shared" si="2"/>
+      <c r="M21" s="23">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N21" s="1">
@@ -2235,15 +2233,15 @@
         <v>2500</v>
       </c>
       <c r="G22" s="11">
-        <f>E22-F22</f>
+        <f t="shared" si="2"/>
         <v>1000</v>
       </c>
       <c r="L22" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2500</v>
       </c>
-      <c r="M22" s="24">
-        <f t="shared" si="2"/>
+      <c r="M22" s="23">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N22" s="1">
@@ -2306,15 +2304,15 @@
         <v>2500</v>
       </c>
       <c r="G23" s="11">
-        <f>E23-F23</f>
+        <f t="shared" si="2"/>
         <v>1000</v>
       </c>
       <c r="L23" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2500</v>
       </c>
-      <c r="M23" s="24">
-        <f t="shared" si="2"/>
+      <c r="M23" s="23">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N23" s="1">
@@ -2377,21 +2375,21 @@
         <v>5000</v>
       </c>
       <c r="G24" s="11">
-        <f>E24-F24</f>
+        <f t="shared" si="2"/>
         <v>1000</v>
       </c>
       <c r="L24" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5000</v>
       </c>
-      <c r="M24" s="24">
-        <f t="shared" si="2"/>
+      <c r="M24" s="23">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N24" s="13">
         <v>1000</v>
       </c>
-      <c r="O24" s="24">
+      <c r="O24" s="23">
         <v>10354</v>
       </c>
       <c r="P24" s="5"/>
@@ -2451,11 +2449,11 @@
         <v>3962</v>
       </c>
       <c r="L25" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3962</v>
       </c>
-      <c r="M25" s="24">
-        <f t="shared" si="2"/>
+      <c r="M25" s="23">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N25" s="1">
@@ -2530,11 +2528,11 @@
         <v>97</v>
       </c>
       <c r="L26" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6280</v>
       </c>
-      <c r="M26" s="24">
-        <f t="shared" si="2"/>
+      <c r="M26" s="23">
+        <f t="shared" si="4"/>
         <v>1092</v>
       </c>
       <c r="N26" s="1">
@@ -2601,11 +2599,11 @@
         <v>1000</v>
       </c>
       <c r="L27" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5000</v>
       </c>
-      <c r="M27" s="24">
-        <f t="shared" si="2"/>
+      <c r="M27" s="23">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N27" s="1">
@@ -2672,11 +2670,11 @@
         <v>1000</v>
       </c>
       <c r="L28" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2500</v>
       </c>
-      <c r="M28" s="24">
-        <f t="shared" si="2"/>
+      <c r="M28" s="23">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N28" s="1">
@@ -2743,11 +2741,11 @@
         <v>1000</v>
       </c>
       <c r="L29" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2500</v>
       </c>
-      <c r="M29" s="24">
-        <f t="shared" si="2"/>
+      <c r="M29" s="23">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N29" s="1">
@@ -2813,11 +2811,11 @@
         <v>500</v>
       </c>
       <c r="L30" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>500</v>
       </c>
-      <c r="M30" s="24">
-        <f t="shared" si="2"/>
+      <c r="M30" s="23">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N30" s="1">
@@ -2884,11 +2882,11 @@
         <v>1000</v>
       </c>
       <c r="L31" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2500</v>
       </c>
-      <c r="M31" s="24">
-        <f t="shared" si="2"/>
+      <c r="M31" s="23">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N31" s="1">
@@ -2955,11 +2953,11 @@
         <v>1000</v>
       </c>
       <c r="L32" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2500</v>
       </c>
-      <c r="M32" s="24">
-        <f t="shared" si="2"/>
+      <c r="M32" s="23">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N32" s="1">
@@ -3016,22 +3014,22 @@
         <v>1043</v>
       </c>
       <c r="E33" s="11">
-        <f>SUM(F33:I33)</f>
+        <f t="shared" ref="E33:E43" si="5">SUM(F33:I33)</f>
         <v>2821</v>
       </c>
       <c r="F33" s="11">
         <v>2351</v>
       </c>
       <c r="G33" s="14">
-        <f>ROUND(0.2*SUM(F33,H33,I33),0)</f>
+        <f t="shared" ref="G33:G40" si="6">ROUND(0.2*SUM(F33,H33,I33),0)</f>
         <v>470</v>
       </c>
       <c r="L33" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2351</v>
       </c>
-      <c r="M33" s="24">
-        <f t="shared" si="2"/>
+      <c r="M33" s="23">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N33" s="1">
@@ -3088,22 +3086,22 @@
         <v>1104</v>
       </c>
       <c r="E34" s="11">
-        <f>SUM(F34:I34)</f>
+        <f t="shared" si="5"/>
         <v>2033</v>
       </c>
       <c r="F34" s="11">
         <v>1694</v>
       </c>
       <c r="G34" s="14">
-        <f>ROUND(0.2*SUM(F34,H34,I34),0)</f>
+        <f t="shared" si="6"/>
         <v>339</v>
       </c>
       <c r="L34" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1694</v>
       </c>
-      <c r="M34" s="24">
-        <f t="shared" si="2"/>
+      <c r="M34" s="23">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N34" s="1">
@@ -3160,12 +3158,12 @@
         <v>645</v>
       </c>
       <c r="E35" s="11">
-        <f>SUM(F35:I35)</f>
+        <f t="shared" si="5"/>
         <v>811</v>
       </c>
       <c r="F35" s="4"/>
       <c r="G35" s="14">
-        <f>ROUND(0.2*SUM(F35,H35,I35),0)</f>
+        <f t="shared" si="6"/>
         <v>135</v>
       </c>
       <c r="H35" s="1">
@@ -3178,8 +3176,8 @@
         <f>SUM(F35,H35,I35)</f>
         <v>676</v>
       </c>
-      <c r="M35" s="24">
-        <f t="shared" si="2"/>
+      <c r="M35" s="23">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N35" s="1">
@@ -3236,12 +3234,12 @@
         <v>642</v>
       </c>
       <c r="E36" s="11">
-        <f>SUM(F36:I36)</f>
+        <f t="shared" si="5"/>
         <v>2868</v>
       </c>
       <c r="F36" s="4"/>
       <c r="G36" s="14">
-        <f>ROUND(0.2*SUM(F36,H36,I36),0)</f>
+        <f t="shared" si="6"/>
         <v>478</v>
       </c>
       <c r="H36" s="1">
@@ -3257,11 +3255,11 @@
         <v>375</v>
       </c>
       <c r="L36" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2390</v>
       </c>
-      <c r="M36" s="24">
-        <f t="shared" si="2"/>
+      <c r="M36" s="23">
+        <f t="shared" si="4"/>
         <v>958</v>
       </c>
       <c r="N36" s="1">
@@ -3318,12 +3316,12 @@
         <v>604</v>
       </c>
       <c r="E37" s="11">
-        <f>SUM(F37:I37)</f>
+        <f t="shared" si="5"/>
         <v>4638</v>
       </c>
       <c r="F37" s="4"/>
       <c r="G37" s="14">
-        <f>ROUND(0.2*SUM(F37,H37,I37),0)</f>
+        <f t="shared" si="6"/>
         <v>773</v>
       </c>
       <c r="H37" s="1">
@@ -3339,11 +3337,11 @@
         <v>250</v>
       </c>
       <c r="L37" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3865</v>
       </c>
-      <c r="M37" s="24">
-        <f t="shared" si="2"/>
+      <c r="M37" s="23">
+        <f t="shared" si="4"/>
         <v>428</v>
       </c>
       <c r="N37" s="1">
@@ -3400,12 +3398,12 @@
         <v>852</v>
       </c>
       <c r="E38" s="11">
-        <f>SUM(F38:I38)</f>
+        <f t="shared" si="5"/>
         <v>5897</v>
       </c>
       <c r="F38" s="4"/>
       <c r="G38" s="14">
-        <f>ROUND(0.2*SUM(F38,H38,I38),0)</f>
+        <f t="shared" si="6"/>
         <v>983</v>
       </c>
       <c r="H38" s="1">
@@ -3421,11 +3419,11 @@
         <v>103</v>
       </c>
       <c r="L38" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4914</v>
       </c>
-      <c r="M38" s="24">
-        <f t="shared" si="2"/>
+      <c r="M38" s="23">
+        <f t="shared" si="4"/>
         <v>584</v>
       </c>
       <c r="N38" s="1">
@@ -3482,12 +3480,12 @@
         <v>499</v>
       </c>
       <c r="E39" s="11">
-        <f>SUM(F39:I39)</f>
+        <f t="shared" si="5"/>
         <v>3876</v>
       </c>
       <c r="F39" s="4"/>
       <c r="G39" s="14">
-        <f>ROUND(0.2*SUM(F39,H39,I39),0)</f>
+        <f t="shared" si="6"/>
         <v>646</v>
       </c>
       <c r="H39" s="1">
@@ -3503,11 +3501,11 @@
         <v>204</v>
       </c>
       <c r="L39" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3230</v>
       </c>
-      <c r="M39" s="24">
-        <f t="shared" si="2"/>
+      <c r="M39" s="23">
+        <f t="shared" si="4"/>
         <v>1615</v>
       </c>
       <c r="N39" s="1">
@@ -3564,12 +3562,12 @@
         <v>538</v>
       </c>
       <c r="E40" s="11">
-        <f>SUM(F40:I40)</f>
+        <f t="shared" si="5"/>
         <v>1488</v>
       </c>
       <c r="F40" s="4"/>
       <c r="G40" s="14">
-        <f>ROUND(0.2*SUM(F40,H40,I40),0)</f>
+        <f t="shared" si="6"/>
         <v>248</v>
       </c>
       <c r="H40" s="1">
@@ -3585,11 +3583,11 @@
         <v>1341</v>
       </c>
       <c r="L40" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1240</v>
       </c>
-      <c r="M40" s="24">
-        <f t="shared" si="2"/>
+      <c r="M40" s="23">
+        <f t="shared" si="4"/>
         <v>2149</v>
       </c>
       <c r="N40" s="1">
@@ -3646,7 +3644,7 @@
         <v>530</v>
       </c>
       <c r="E41" s="11">
-        <f>SUM(F41:I41)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F41" s="4"/>
@@ -3666,11 +3664,11 @@
         <v>0</v>
       </c>
       <c r="L41" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M41" s="24">
-        <f t="shared" si="2"/>
+      <c r="M41" s="23">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N41" s="1">
@@ -3727,7 +3725,7 @@
         <v>473</v>
       </c>
       <c r="E42" s="11">
-        <f>SUM(F42:I42)</f>
+        <f t="shared" si="5"/>
         <v>762</v>
       </c>
       <c r="F42" s="4"/>
@@ -3749,11 +3747,11 @@
         <v>120</v>
       </c>
       <c r="L42" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>762</v>
       </c>
-      <c r="M42" s="24">
-        <f t="shared" si="2"/>
+      <c r="M42" s="23">
+        <f t="shared" si="4"/>
         <v>141</v>
       </c>
       <c r="N42" s="1">
@@ -3810,7 +3808,7 @@
         <v>550</v>
       </c>
       <c r="E43" s="11">
-        <f>SUM(F43:I43)</f>
+        <f t="shared" si="5"/>
         <v>1072</v>
       </c>
       <c r="F43" s="4"/>
@@ -3832,11 +3830,11 @@
         <v>381</v>
       </c>
       <c r="L43" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1072</v>
       </c>
-      <c r="M43" s="24">
-        <f t="shared" si="2"/>
+      <c r="M43" s="23">
+        <f t="shared" si="4"/>
         <v>451</v>
       </c>
       <c r="N43" s="1">
@@ -3882,7 +3880,7 @@
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
       <c r="L44" s="5"/>
-      <c r="M44" s="25"/>
+      <c r="M44" s="24"/>
       <c r="R44" s="5"/>
       <c r="S44" s="5"/>
       <c r="T44" s="5"/>
@@ -3909,11 +3907,20 @@
       <c r="BI44" s="7"/>
     </row>
     <row r="45" spans="1:61" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D45" s="35" t="s">
+        <v>14</v>
+      </c>
       <c r="E45" s="15" t="s">
         <v>13</v>
       </c>
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
+      <c r="N45" s="13" t="s">
+        <v>20</v>
+      </c>
       <c r="AL45" s="7"/>
       <c r="AM45" s="7"/>
       <c r="AN45" s="7"/>
@@ -3928,15 +3935,11 @@
       <c r="BI45" s="7"/>
     </row>
     <row r="46" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A46" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="B46" s="16"/>
-      <c r="C46" s="16"/>
-      <c r="D46" s="16"/>
-      <c r="E46" s="10" t="s">
-        <v>15</v>
-      </c>
+      <c r="E46" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F46" s="4"/>
+      <c r="G46" s="4"/>
       <c r="AL46" s="7"/>
       <c r="AM46" s="7"/>
       <c r="AN46" s="7"/>
@@ -3951,11 +3954,11 @@
       <c r="BI46" s="7"/>
     </row>
     <row r="47" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A47" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>17</v>
+      <c r="B47" s="35"/>
+      <c r="C47" s="35"/>
+      <c r="D47" s="35"/>
+      <c r="E47" s="10" t="s">
+        <v>15</v>
       </c>
       <c r="AL47" s="7"/>
       <c r="AM47" s="7"/>
@@ -3971,115 +3974,122 @@
       <c r="BI47" s="7"/>
     </row>
     <row r="48" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A48" s="23" t="s">
-        <v>18</v>
-      </c>
       <c r="E48" s="1" t="s">
-        <v>19</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="AL48" s="7"/>
+      <c r="AM48" s="7"/>
+      <c r="AN48" s="7"/>
+      <c r="AO48" s="7"/>
+      <c r="AP48" s="7"/>
+      <c r="AQ48" s="7"/>
+      <c r="AS48" s="7"/>
+      <c r="AU48" s="7"/>
+      <c r="AW48" s="7"/>
+      <c r="AY48" s="7"/>
       <c r="BD48" s="7"/>
       <c r="BI48" s="7"/>
     </row>
-    <row r="49" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A49" s="17" t="s">
-        <v>20</v>
-      </c>
+    <row r="49" spans="2:61" x14ac:dyDescent="0.2">
       <c r="E49" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="BD49" s="7"/>
       <c r="BI49" s="7"/>
     </row>
-    <row r="50" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A50" s="13" t="s">
-        <v>22</v>
-      </c>
+    <row r="50" spans="2:61" x14ac:dyDescent="0.2">
       <c r="E50" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="BD50" s="7"/>
       <c r="BI50" s="7"/>
     </row>
-    <row r="51" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:61" x14ac:dyDescent="0.2">
       <c r="E51" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="BD51" s="7"/>
       <c r="BI51" s="7"/>
     </row>
-    <row r="52" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:61" x14ac:dyDescent="0.2">
       <c r="E52" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="BD52" s="7"/>
       <c r="BI52" s="7"/>
     </row>
-    <row r="53" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="E53" s="18" t="s">
-        <v>26</v>
+    <row r="53" spans="2:61" x14ac:dyDescent="0.2">
+      <c r="E53" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="BD53" s="7"/>
       <c r="BI53" s="7"/>
     </row>
-    <row r="54" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:61" x14ac:dyDescent="0.2">
+      <c r="E54" s="17" t="s">
+        <v>24</v>
+      </c>
       <c r="BD54" s="7"/>
       <c r="BI54" s="7"/>
     </row>
-    <row r="55" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:61" x14ac:dyDescent="0.2">
+      <c r="E55" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="BD55" s="7"/>
       <c r="BI55" s="7"/>
     </row>
-    <row r="56" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:61" x14ac:dyDescent="0.2">
       <c r="BD56" s="7"/>
       <c r="BI56" s="7"/>
     </row>
-    <row r="57" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:61" x14ac:dyDescent="0.2">
       <c r="BD57" s="7"/>
       <c r="BI57" s="7"/>
     </row>
-    <row r="58" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:61" x14ac:dyDescent="0.2">
       <c r="BD58" s="7"/>
       <c r="BI58" s="7"/>
     </row>
-    <row r="59" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:61" x14ac:dyDescent="0.2">
       <c r="BD59" s="7"/>
       <c r="BI59" s="7"/>
     </row>
-    <row r="60" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="B60" s="2"/>
-      <c r="C60" s="2"/>
-      <c r="D60" s="2"/>
-      <c r="E60" s="2"/>
-      <c r="F60" s="2"/>
-      <c r="G60" s="2"/>
-      <c r="H60" s="2"/>
-      <c r="I60" s="2"/>
-      <c r="J60" s="2"/>
-      <c r="K60" s="2"/>
-      <c r="L60" s="2"/>
-      <c r="M60" s="19"/>
-      <c r="N60" s="2"/>
-      <c r="O60" s="2"/>
-      <c r="P60" s="2"/>
-      <c r="S60" s="3"/>
-      <c r="T60" s="3"/>
-      <c r="U60" s="3"/>
-      <c r="W60" s="3"/>
-      <c r="AI60" s="3"/>
-    </row>
-    <row r="61" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="BD61" s="7"/>
-      <c r="BI61" s="7"/>
-    </row>
-    <row r="62" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:61" x14ac:dyDescent="0.2">
+      <c r="BD60" s="7"/>
+      <c r="BI60" s="7"/>
+    </row>
+    <row r="61" spans="2:61" x14ac:dyDescent="0.2">
+      <c r="B61" s="2"/>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2"/>
+      <c r="E61" s="2"/>
+      <c r="F61" s="2"/>
+      <c r="G61" s="2"/>
+      <c r="H61" s="2"/>
+      <c r="I61" s="2"/>
+      <c r="J61" s="2"/>
+      <c r="K61" s="2"/>
+      <c r="L61" s="2"/>
+      <c r="M61" s="18"/>
+      <c r="N61" s="2"/>
+      <c r="O61" s="2"/>
+      <c r="P61" s="2"/>
+      <c r="S61" s="3"/>
+      <c r="T61" s="3"/>
+      <c r="U61" s="3"/>
+      <c r="W61" s="3"/>
+      <c r="AI61" s="3"/>
+    </row>
+    <row r="62" spans="2:61" x14ac:dyDescent="0.2">
       <c r="BD62" s="7"/>
       <c r="BI62" s="7"/>
     </row>
-    <row r="63" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:61" x14ac:dyDescent="0.2">
       <c r="BD63" s="7"/>
       <c r="BI63" s="7"/>
     </row>
-    <row r="64" spans="1:61" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:61" x14ac:dyDescent="0.2">
       <c r="BD64" s="7"/>
       <c r="BI64" s="7"/>
     </row>
@@ -4485,6 +4495,7 @@
     </row>
     <row r="165" spans="56:61" x14ac:dyDescent="0.2">
       <c r="BD165" s="7"/>
+      <c r="BI165" s="7"/>
     </row>
     <row r="166" spans="56:61" x14ac:dyDescent="0.2">
       <c r="BD166" s="7"/>
@@ -4546,10 +4557,10 @@
     <row r="185" spans="56:56" x14ac:dyDescent="0.2">
       <c r="BD185" s="7"/>
     </row>
+    <row r="186" spans="56:56" x14ac:dyDescent="0.2">
+      <c r="BD186" s="7"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A46:D46"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update freshwater catch formatting
</commit_message>
<xml_diff>
--- a/data-raw/freshwater-catch.xlsx
+++ b/data-raw/freshwater-catch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\skrunchy2025\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFB62E85-4C26-4001-8636-1A5E3CC34E41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54F75AB3-113A-4B32-BCE4-4FEAAAC54D0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E0CDEE87-6CC2-4107-81B9-F1AD4EA649A7}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E0CDEE87-6CC2-4107-81B9-F1AD4EA649A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -132,7 +132,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -168,12 +168,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -245,7 +239,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -299,17 +293,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="6" fillId="3" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
@@ -633,8 +616,8 @@
   <dimension ref="A1:BI186"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A46" sqref="A46"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1121,78 +1104,78 @@
       <c r="BD6" s="7"/>
       <c r="BI6" s="7"/>
     </row>
-    <row r="7" spans="1:61" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="28">
+    <row r="7" spans="1:61" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
         <v>1984</v>
       </c>
-      <c r="B7" s="28">
+      <c r="B7" s="1">
         <v>587</v>
       </c>
-      <c r="C7" s="28">
+      <c r="C7" s="1">
         <v>153</v>
       </c>
-      <c r="D7" s="28">
+      <c r="D7" s="1">
         <f t="shared" si="0"/>
         <v>740</v>
       </c>
-      <c r="E7" s="29">
+      <c r="E7" s="6">
         <v>2976</v>
       </c>
-      <c r="F7" s="29">
+      <c r="F7" s="6">
         <f t="shared" si="1"/>
         <v>1984</v>
       </c>
-      <c r="G7" s="29">
+      <c r="G7" s="6">
         <f t="shared" si="2"/>
         <v>992</v>
       </c>
-      <c r="L7" s="30">
+      <c r="L7" s="7">
         <f t="shared" si="3"/>
         <v>1984</v>
       </c>
-      <c r="M7" s="31">
+      <c r="M7" s="23">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="N7" s="28">
+      <c r="N7" s="1">
         <v>1568</v>
       </c>
-      <c r="O7" s="30">
+      <c r="O7" s="7">
         <v>7900</v>
       </c>
-      <c r="P7" s="32"/>
-      <c r="Q7" s="32"/>
-      <c r="R7" s="32"/>
-      <c r="S7" s="32"/>
-      <c r="T7" s="30"/>
-      <c r="U7" s="30"/>
-      <c r="V7" s="30"/>
-      <c r="W7" s="30"/>
-      <c r="X7" s="30"/>
-      <c r="Y7" s="33"/>
-      <c r="Z7" s="33"/>
-      <c r="AA7" s="33"/>
-      <c r="AB7" s="33"/>
-      <c r="AC7" s="33"/>
-      <c r="AD7" s="30"/>
-      <c r="AE7" s="30"/>
-      <c r="AF7" s="30"/>
-      <c r="AG7" s="30"/>
-      <c r="AH7" s="30"/>
-      <c r="AI7" s="30"/>
-      <c r="AJ7" s="34"/>
-      <c r="AL7" s="30"/>
-      <c r="AM7" s="30"/>
-      <c r="AN7" s="30"/>
-      <c r="AO7" s="30"/>
-      <c r="AP7" s="30"/>
-      <c r="AQ7" s="30"/>
-      <c r="AS7" s="30"/>
-      <c r="AU7" s="30"/>
-      <c r="AW7" s="30"/>
-      <c r="AY7" s="30"/>
-      <c r="BD7" s="30"/>
-      <c r="BI7" s="30"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="5"/>
+      <c r="S7" s="5"/>
+      <c r="T7" s="7"/>
+      <c r="U7" s="7"/>
+      <c r="V7" s="7"/>
+      <c r="W7" s="7"/>
+      <c r="X7" s="7"/>
+      <c r="Y7" s="8"/>
+      <c r="Z7" s="8"/>
+      <c r="AA7" s="8"/>
+      <c r="AB7" s="8"/>
+      <c r="AC7" s="8"/>
+      <c r="AD7" s="7"/>
+      <c r="AE7" s="7"/>
+      <c r="AF7" s="7"/>
+      <c r="AG7" s="7"/>
+      <c r="AH7" s="7"/>
+      <c r="AI7" s="7"/>
+      <c r="AJ7" s="9"/>
+      <c r="AL7" s="7"/>
+      <c r="AM7" s="7"/>
+      <c r="AN7" s="7"/>
+      <c r="AO7" s="7"/>
+      <c r="AP7" s="7"/>
+      <c r="AQ7" s="7"/>
+      <c r="AS7" s="7"/>
+      <c r="AU7" s="7"/>
+      <c r="AW7" s="7"/>
+      <c r="AY7" s="7"/>
+      <c r="BD7" s="7"/>
+      <c r="BI7" s="7"/>
     </row>
     <row r="8" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
@@ -3910,7 +3893,7 @@
       <c r="A45" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D45" s="35" t="s">
+      <c r="D45" s="28" t="s">
         <v>14</v>
       </c>
       <c r="E45" s="15" t="s">
@@ -3954,9 +3937,9 @@
       <c r="BI46" s="7"/>
     </row>
     <row r="47" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="B47" s="35"/>
-      <c r="C47" s="35"/>
-      <c r="D47" s="35"/>
+      <c r="B47" s="28"/>
+      <c r="C47" s="28"/>
+      <c r="D47" s="28"/>
       <c r="E47" s="10" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
Add 2021-2024 tyee catch data to freshwater-catch file, update readme
</commit_message>
<xml_diff>
--- a/data-raw/freshwater-catch.xlsx
+++ b/data-raw/freshwater-catch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\skrunchy2025\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54F75AB3-113A-4B32-BCE4-4FEAAAC54D0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{776C660A-5AA6-438F-BCE2-B9F1306EFBA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E0CDEE87-6CC2-4107-81B9-F1AD4EA649A7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E0CDEE87-6CC2-4107-81B9-F1AD4EA649A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="32">
   <si>
     <t>Year</t>
   </si>
@@ -123,6 +123,15 @@
   </si>
   <si>
     <t>Notes</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Winther et al. 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LW </t>
   </si>
 </sst>
 </file>
@@ -613,11 +622,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35E3952C-60AA-4AE7-A274-2D9A331D3C7B}">
-  <dimension ref="A1:BI186"/>
+  <dimension ref="A1:BI190"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K18" sqref="K18"/>
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M39" sqref="M39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -627,7 +636,9 @@
     <col min="4" max="4" width="7.140625" style="1" customWidth="1"/>
     <col min="5" max="12" width="8.7109375" style="1"/>
     <col min="13" max="13" width="8.42578125" style="19" customWidth="1"/>
-    <col min="14" max="22" width="7.5703125" style="1" customWidth="1"/>
+    <col min="14" max="15" width="7.5703125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="20.28515625" style="1" customWidth="1"/>
+    <col min="17" max="22" width="7.5703125" style="1" customWidth="1"/>
     <col min="23" max="24" width="8.85546875" style="1" customWidth="1"/>
     <col min="25" max="28" width="7.5703125" style="1" customWidth="1"/>
     <col min="29" max="29" width="8.140625" style="1" customWidth="1"/>
@@ -697,7 +708,9 @@
       <c r="O1" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="2"/>
+      <c r="P1" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="Q1" s="18"/>
       <c r="R1" s="18"/>
       <c r="S1" s="18"/>
@@ -782,7 +795,9 @@
       <c r="O2" s="7">
         <v>2500</v>
       </c>
-      <c r="P2" s="7"/>
+      <c r="P2" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="Q2" s="7"/>
       <c r="R2" s="7"/>
       <c r="S2" s="7"/>
@@ -841,7 +856,7 @@
         <v>1208</v>
       </c>
       <c r="L3" s="7">
-        <f t="shared" ref="L3:L43" si="3">SUM(F3,H3,I3)</f>
+        <f t="shared" ref="L3:L42" si="3">SUM(F3,H3,I3)</f>
         <v>2417</v>
       </c>
       <c r="M3" s="23">
@@ -854,7 +869,9 @@
       <c r="O3" s="7">
         <v>6060</v>
       </c>
-      <c r="P3" s="5"/>
+      <c r="P3" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="Q3" s="5"/>
       <c r="R3" s="5"/>
       <c r="S3" s="5"/>
@@ -926,7 +943,9 @@
       <c r="O4" s="7">
         <v>7621</v>
       </c>
-      <c r="P4" s="5"/>
+      <c r="P4" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="Q4" s="5"/>
       <c r="R4" s="5"/>
       <c r="S4" s="5"/>
@@ -998,7 +1017,9 @@
       <c r="O5" s="7">
         <v>9200</v>
       </c>
-      <c r="P5" s="5"/>
+      <c r="P5" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="Q5" s="5"/>
       <c r="R5" s="5"/>
       <c r="S5" s="5"/>
@@ -1070,7 +1091,9 @@
       <c r="O6" s="7">
         <v>8300</v>
       </c>
-      <c r="P6" s="5"/>
+      <c r="P6" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="Q6" s="5"/>
       <c r="R6" s="5"/>
       <c r="S6" s="5"/>
@@ -1143,7 +1166,9 @@
       <c r="O7" s="7">
         <v>7900</v>
       </c>
-      <c r="P7" s="5"/>
+      <c r="P7" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="Q7" s="5"/>
       <c r="R7" s="5"/>
       <c r="S7" s="5"/>
@@ -1216,7 +1241,9 @@
       <c r="O8" s="7">
         <v>10300</v>
       </c>
-      <c r="P8" s="5"/>
+      <c r="P8" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="Q8" s="5"/>
       <c r="R8" s="5"/>
       <c r="S8" s="5"/>
@@ -1289,7 +1316,9 @@
       <c r="O9" s="7">
         <v>10653</v>
       </c>
-      <c r="P9" s="5"/>
+      <c r="P9" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="Q9" s="5"/>
       <c r="R9" s="5"/>
       <c r="S9" s="5"/>
@@ -1362,7 +1391,9 @@
       <c r="O10" s="7">
         <v>7900</v>
       </c>
-      <c r="P10" s="5"/>
+      <c r="P10" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="Q10" s="5"/>
       <c r="R10" s="5"/>
       <c r="S10" s="5"/>
@@ -1435,7 +1466,9 @@
       <c r="O11" s="7">
         <v>13700</v>
       </c>
-      <c r="P11" s="5"/>
+      <c r="P11" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="Q11" s="5"/>
       <c r="R11" s="5"/>
       <c r="S11" s="5"/>
@@ -1508,7 +1541,9 @@
       <c r="O12" s="7">
         <v>9400</v>
       </c>
-      <c r="P12" s="5"/>
+      <c r="P12" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="Q12" s="5"/>
       <c r="R12" s="5"/>
       <c r="S12" s="5"/>
@@ -1581,7 +1616,9 @@
       <c r="O13" s="7">
         <v>17855</v>
       </c>
-      <c r="P13" s="5"/>
+      <c r="P13" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="Q13" s="5"/>
       <c r="R13" s="5"/>
       <c r="S13" s="5"/>
@@ -1654,7 +1691,9 @@
       <c r="O14" s="7">
         <v>11700</v>
       </c>
-      <c r="P14" s="5"/>
+      <c r="P14" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="Q14" s="5"/>
       <c r="R14" s="5"/>
       <c r="S14" s="5"/>
@@ -1727,7 +1766,9 @@
       <c r="O15" s="7">
         <v>11361</v>
       </c>
-      <c r="P15" s="5"/>
+      <c r="P15" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="Q15" s="5"/>
       <c r="R15" s="5"/>
       <c r="S15" s="5"/>
@@ -1800,7 +1841,9 @@
       <c r="O16" s="7">
         <v>9569</v>
       </c>
-      <c r="P16" s="5"/>
+      <c r="P16" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="Q16" s="5"/>
       <c r="R16" s="5"/>
       <c r="S16" s="5"/>
@@ -1873,7 +1916,9 @@
       <c r="O17" s="7">
         <v>8140</v>
       </c>
-      <c r="P17" s="5"/>
+      <c r="P17" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="Q17" s="5"/>
       <c r="R17" s="5"/>
       <c r="S17" s="5"/>
@@ -1946,7 +1991,9 @@
       <c r="O18" s="7">
         <v>5724</v>
       </c>
-      <c r="P18" s="5"/>
+      <c r="P18" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="Q18" s="5"/>
       <c r="R18" s="5"/>
       <c r="S18" s="5"/>
@@ -2019,7 +2066,9 @@
       <c r="O19" s="7">
         <v>4828</v>
       </c>
-      <c r="P19" s="5"/>
+      <c r="P19" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="Q19" s="5"/>
       <c r="R19" s="5"/>
       <c r="S19" s="5"/>
@@ -2091,7 +2140,9 @@
       <c r="O20" s="7">
         <v>6289</v>
       </c>
-      <c r="P20" s="5"/>
+      <c r="P20" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="Q20" s="5"/>
       <c r="R20" s="5"/>
       <c r="S20" s="5"/>
@@ -2162,7 +2213,9 @@
       <c r="O21" s="7">
         <v>9783</v>
       </c>
-      <c r="P21" s="5"/>
+      <c r="P21" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="Q21" s="5"/>
       <c r="R21" s="5"/>
       <c r="S21" s="5"/>
@@ -2233,7 +2286,9 @@
       <c r="O22" s="7">
         <v>15345</v>
       </c>
-      <c r="P22" s="5"/>
+      <c r="P22" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="Q22" s="5"/>
       <c r="R22" s="5"/>
       <c r="S22" s="5"/>
@@ -2304,7 +2359,9 @@
       <c r="O23" s="7">
         <v>12296</v>
       </c>
-      <c r="P23" s="5"/>
+      <c r="P23" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="Q23" s="5"/>
       <c r="R23" s="5"/>
       <c r="S23" s="5"/>
@@ -2375,7 +2432,9 @@
       <c r="O24" s="23">
         <v>10354</v>
       </c>
-      <c r="P24" s="5"/>
+      <c r="P24" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="Q24" s="5"/>
       <c r="R24" s="5"/>
       <c r="S24" s="5"/>
@@ -2445,7 +2504,9 @@
       <c r="O25" s="7">
         <v>6207</v>
       </c>
-      <c r="P25" s="5"/>
+      <c r="P25" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="Q25" s="5"/>
       <c r="R25" s="5"/>
       <c r="S25" s="5"/>
@@ -2524,7 +2585,9 @@
       <c r="O26" s="7">
         <v>10472</v>
       </c>
-      <c r="P26" s="5"/>
+      <c r="P26" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="Q26" s="5"/>
       <c r="R26" s="5"/>
       <c r="S26" s="5"/>
@@ -2595,7 +2658,9 @@
       <c r="O27" s="7">
         <v>10924</v>
       </c>
-      <c r="P27" s="5"/>
+      <c r="P27" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="Q27" s="5"/>
       <c r="R27" s="5"/>
       <c r="S27" s="5"/>
@@ -2666,7 +2731,9 @@
       <c r="O28" s="7">
         <v>6939</v>
       </c>
-      <c r="P28" s="5"/>
+      <c r="P28" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="Q28" s="5"/>
       <c r="R28" s="5"/>
       <c r="S28" s="5"/>
@@ -2737,7 +2804,9 @@
       <c r="O29" s="7">
         <v>6235</v>
       </c>
-      <c r="P29" s="5"/>
+      <c r="P29" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="Q29" s="5"/>
       <c r="R29" s="5"/>
       <c r="S29" s="5"/>
@@ -2807,7 +2876,9 @@
       <c r="O30" s="7">
         <v>4816</v>
       </c>
-      <c r="P30" s="5"/>
+      <c r="P30" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="Q30" s="5"/>
       <c r="R30" s="5"/>
       <c r="S30" s="5"/>
@@ -2878,7 +2949,9 @@
       <c r="O31" s="7">
         <v>7887</v>
       </c>
-      <c r="P31" s="5"/>
+      <c r="P31" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="Q31" s="5"/>
       <c r="R31" s="5"/>
       <c r="S31" s="5"/>
@@ -2949,7 +3022,9 @@
       <c r="O32" s="7">
         <v>5576</v>
       </c>
-      <c r="P32" s="5"/>
+      <c r="P32" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="Q32" s="5"/>
       <c r="R32" s="5"/>
       <c r="S32" s="5"/>
@@ -3021,7 +3096,9 @@
       <c r="O33" s="7">
         <v>6115</v>
       </c>
-      <c r="P33" s="5"/>
+      <c r="P33" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="Q33" s="5"/>
       <c r="R33" s="5"/>
       <c r="S33" s="5"/>
@@ -3093,7 +3170,9 @@
       <c r="O34" s="7">
         <v>3764</v>
       </c>
-      <c r="P34" s="5"/>
+      <c r="P34" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="Q34" s="5"/>
       <c r="R34" s="5"/>
       <c r="S34" s="5"/>
@@ -3169,7 +3248,9 @@
       <c r="O35" s="7">
         <v>2533</v>
       </c>
-      <c r="P35" s="5"/>
+      <c r="P35" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="Q35" s="5"/>
       <c r="R35" s="5"/>
       <c r="S35" s="5"/>
@@ -3251,7 +3332,9 @@
       <c r="O36" s="7">
         <v>2142</v>
       </c>
-      <c r="P36" s="5"/>
+      <c r="P36" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="Q36" s="5"/>
       <c r="R36" s="5"/>
       <c r="S36" s="5"/>
@@ -3333,7 +3416,9 @@
       <c r="O37" s="7">
         <v>3365</v>
       </c>
-      <c r="P37" s="5"/>
+      <c r="P37" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="Q37" s="5"/>
       <c r="R37" s="5"/>
       <c r="S37" s="5"/>
@@ -3415,7 +3500,9 @@
       <c r="O38" s="7">
         <v>5850</v>
       </c>
-      <c r="P38" s="5"/>
+      <c r="P38" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="Q38" s="5"/>
       <c r="R38" s="5"/>
       <c r="S38" s="5"/>
@@ -3497,7 +3584,9 @@
       <c r="O39" s="7">
         <v>3532</v>
       </c>
-      <c r="P39" s="5"/>
+      <c r="P39" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="Q39" s="5"/>
       <c r="R39" s="5"/>
       <c r="S39" s="5"/>
@@ -3579,7 +3668,9 @@
       <c r="O40" s="7">
         <v>4474</v>
       </c>
-      <c r="P40" s="5"/>
+      <c r="P40" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="Q40" s="5"/>
       <c r="R40" s="5"/>
       <c r="S40" s="5"/>
@@ -3660,7 +3751,9 @@
       <c r="O41" s="7">
         <v>5983</v>
       </c>
-      <c r="P41" s="5"/>
+      <c r="P41" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="Q41" s="5"/>
       <c r="R41" s="5"/>
       <c r="S41" s="5"/>
@@ -3743,7 +3836,9 @@
       <c r="O42" s="7">
         <v>4460</v>
       </c>
-      <c r="P42" s="5"/>
+      <c r="P42" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="Q42" s="5"/>
       <c r="R42" s="5"/>
       <c r="S42" s="5"/>
@@ -3813,7 +3908,7 @@
         <v>381</v>
       </c>
       <c r="L43" s="7">
-        <f t="shared" si="3"/>
+        <f>SUM(F43,H43,I43)</f>
         <v>1072</v>
       </c>
       <c r="M43" s="23">
@@ -3826,7 +3921,9 @@
       <c r="O43" s="7">
         <v>3904</v>
       </c>
-      <c r="P43" s="5"/>
+      <c r="P43" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="Q43" s="5"/>
       <c r="R43" s="5"/>
       <c r="S43" s="5"/>
@@ -3860,22 +3957,46 @@
       <c r="BI43" s="7"/>
     </row>
     <row r="44" spans="1:61" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
+        <v>2021</v>
+      </c>
+      <c r="B44" s="1">
+        <v>320</v>
+      </c>
+      <c r="C44" s="1">
+        <v>162</v>
+      </c>
+      <c r="D44" s="1">
+        <v>482</v>
+      </c>
+      <c r="E44" s="11"/>
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
-      <c r="L44" s="5"/>
-      <c r="M44" s="24"/>
+      <c r="L44" s="7"/>
+      <c r="M44" s="23"/>
+      <c r="O44" s="7"/>
+      <c r="P44" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q44" s="5"/>
       <c r="R44" s="5"/>
       <c r="S44" s="5"/>
-      <c r="T44" s="5"/>
-      <c r="U44" s="5"/>
-      <c r="V44" s="5"/>
-      <c r="W44" s="5"/>
-      <c r="X44" s="5"/>
+      <c r="T44" s="7"/>
+      <c r="U44" s="7"/>
+      <c r="V44" s="7"/>
+      <c r="W44" s="7"/>
+      <c r="X44" s="7"/>
       <c r="Y44" s="8"/>
       <c r="Z44" s="8"/>
       <c r="AA44" s="8"/>
       <c r="AB44" s="8"/>
       <c r="AC44" s="8"/>
+      <c r="AD44" s="7"/>
+      <c r="AE44" s="7"/>
+      <c r="AF44" s="7"/>
+      <c r="AG44" s="7"/>
+      <c r="AH44" s="7"/>
+      <c r="AI44" s="7"/>
       <c r="AL44" s="7"/>
       <c r="AM44" s="7"/>
       <c r="AN44" s="7"/>
@@ -3890,20 +4011,46 @@
       <c r="BI44" s="7"/>
     </row>
     <row r="45" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D45" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="E45" s="15" t="s">
-        <v>13</v>
-      </c>
+      <c r="A45" s="1">
+        <v>2022</v>
+      </c>
+      <c r="B45" s="1">
+        <v>672</v>
+      </c>
+      <c r="C45" s="1">
+        <v>231</v>
+      </c>
+      <c r="D45" s="1">
+        <v>903</v>
+      </c>
+      <c r="E45" s="11"/>
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
-      <c r="N45" s="13" t="s">
-        <v>20</v>
-      </c>
+      <c r="L45" s="7"/>
+      <c r="M45" s="23"/>
+      <c r="O45" s="7"/>
+      <c r="P45" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q45" s="5"/>
+      <c r="R45" s="5"/>
+      <c r="S45" s="5"/>
+      <c r="T45" s="7"/>
+      <c r="U45" s="7"/>
+      <c r="V45" s="7"/>
+      <c r="W45" s="7"/>
+      <c r="X45" s="7"/>
+      <c r="Y45" s="8"/>
+      <c r="Z45" s="8"/>
+      <c r="AA45" s="8"/>
+      <c r="AB45" s="8"/>
+      <c r="AC45" s="8"/>
+      <c r="AD45" s="7"/>
+      <c r="AE45" s="7"/>
+      <c r="AF45" s="7"/>
+      <c r="AG45" s="7"/>
+      <c r="AH45" s="7"/>
+      <c r="AI45" s="7"/>
       <c r="AL45" s="7"/>
       <c r="AM45" s="7"/>
       <c r="AN45" s="7"/>
@@ -3918,11 +4065,46 @@
       <c r="BI45" s="7"/>
     </row>
     <row r="46" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="E46" s="16" t="s">
-        <v>18</v>
-      </c>
+      <c r="A46" s="1">
+        <v>2023</v>
+      </c>
+      <c r="B46" s="1">
+        <v>392</v>
+      </c>
+      <c r="C46" s="1">
+        <v>254</v>
+      </c>
+      <c r="D46" s="1">
+        <v>646</v>
+      </c>
+      <c r="E46" s="11"/>
       <c r="F46" s="4"/>
       <c r="G46" s="4"/>
+      <c r="L46" s="7"/>
+      <c r="M46" s="23"/>
+      <c r="O46" s="7"/>
+      <c r="P46" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q46" s="5"/>
+      <c r="R46" s="5"/>
+      <c r="S46" s="5"/>
+      <c r="T46" s="7"/>
+      <c r="U46" s="7"/>
+      <c r="V46" s="7"/>
+      <c r="W46" s="7"/>
+      <c r="X46" s="7"/>
+      <c r="Y46" s="8"/>
+      <c r="Z46" s="8"/>
+      <c r="AA46" s="8"/>
+      <c r="AB46" s="8"/>
+      <c r="AC46" s="8"/>
+      <c r="AD46" s="7"/>
+      <c r="AE46" s="7"/>
+      <c r="AF46" s="7"/>
+      <c r="AG46" s="7"/>
+      <c r="AH46" s="7"/>
+      <c r="AI46" s="7"/>
       <c r="AL46" s="7"/>
       <c r="AM46" s="7"/>
       <c r="AN46" s="7"/>
@@ -3937,12 +4119,46 @@
       <c r="BI46" s="7"/>
     </row>
     <row r="47" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="B47" s="28"/>
-      <c r="C47" s="28"/>
-      <c r="D47" s="28"/>
-      <c r="E47" s="10" t="s">
-        <v>15</v>
-      </c>
+      <c r="A47" s="1">
+        <v>2024</v>
+      </c>
+      <c r="B47" s="1">
+        <v>283</v>
+      </c>
+      <c r="C47" s="1">
+        <v>199</v>
+      </c>
+      <c r="D47" s="1">
+        <v>482</v>
+      </c>
+      <c r="E47" s="11"/>
+      <c r="F47" s="4"/>
+      <c r="G47" s="4"/>
+      <c r="L47" s="7"/>
+      <c r="M47" s="23"/>
+      <c r="O47" s="7"/>
+      <c r="P47" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q47" s="5"/>
+      <c r="R47" s="5"/>
+      <c r="S47" s="5"/>
+      <c r="T47" s="7"/>
+      <c r="U47" s="7"/>
+      <c r="V47" s="7"/>
+      <c r="W47" s="7"/>
+      <c r="X47" s="7"/>
+      <c r="Y47" s="8"/>
+      <c r="Z47" s="8"/>
+      <c r="AA47" s="8"/>
+      <c r="AB47" s="8"/>
+      <c r="AC47" s="8"/>
+      <c r="AD47" s="7"/>
+      <c r="AE47" s="7"/>
+      <c r="AF47" s="7"/>
+      <c r="AG47" s="7"/>
+      <c r="AH47" s="7"/>
+      <c r="AI47" s="7"/>
       <c r="AL47" s="7"/>
       <c r="AM47" s="7"/>
       <c r="AN47" s="7"/>
@@ -3957,9 +4173,22 @@
       <c r="BI47" s="7"/>
     </row>
     <row r="48" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="E48" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="F48" s="4"/>
+      <c r="G48" s="4"/>
+      <c r="L48" s="5"/>
+      <c r="M48" s="24"/>
+      <c r="R48" s="5"/>
+      <c r="S48" s="5"/>
+      <c r="T48" s="5"/>
+      <c r="U48" s="5"/>
+      <c r="V48" s="5"/>
+      <c r="W48" s="5"/>
+      <c r="X48" s="5"/>
+      <c r="Y48" s="8"/>
+      <c r="Z48" s="8"/>
+      <c r="AA48" s="8"/>
+      <c r="AB48" s="8"/>
+      <c r="AC48" s="8"/>
       <c r="AL48" s="7"/>
       <c r="AM48" s="7"/>
       <c r="AN48" s="7"/>
@@ -3973,170 +4202,238 @@
       <c r="BD48" s="7"/>
       <c r="BI48" s="7"/>
     </row>
-    <row r="49" spans="2:61" x14ac:dyDescent="0.2">
-      <c r="E49" s="1" t="s">
-        <v>17</v>
-      </c>
+    <row r="49" spans="1:61" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D49" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="E49" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F49" s="4"/>
+      <c r="G49" s="4"/>
+      <c r="N49" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="AL49" s="7"/>
+      <c r="AM49" s="7"/>
+      <c r="AN49" s="7"/>
+      <c r="AO49" s="7"/>
+      <c r="AP49" s="7"/>
+      <c r="AQ49" s="7"/>
+      <c r="AS49" s="7"/>
+      <c r="AU49" s="7"/>
+      <c r="AW49" s="7"/>
+      <c r="AY49" s="7"/>
       <c r="BD49" s="7"/>
       <c r="BI49" s="7"/>
     </row>
-    <row r="50" spans="2:61" x14ac:dyDescent="0.2">
-      <c r="E50" s="1" t="s">
-        <v>19</v>
-      </c>
+    <row r="50" spans="1:61" x14ac:dyDescent="0.2">
+      <c r="E50" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F50" s="4"/>
+      <c r="G50" s="4"/>
+      <c r="AL50" s="7"/>
+      <c r="AM50" s="7"/>
+      <c r="AN50" s="7"/>
+      <c r="AO50" s="7"/>
+      <c r="AP50" s="7"/>
+      <c r="AQ50" s="7"/>
+      <c r="AS50" s="7"/>
+      <c r="AU50" s="7"/>
+      <c r="AW50" s="7"/>
+      <c r="AY50" s="7"/>
       <c r="BD50" s="7"/>
       <c r="BI50" s="7"/>
     </row>
-    <row r="51" spans="2:61" x14ac:dyDescent="0.2">
-      <c r="E51" s="1" t="s">
-        <v>21</v>
-      </c>
+    <row r="51" spans="1:61" x14ac:dyDescent="0.2">
+      <c r="B51" s="28"/>
+      <c r="C51" s="28"/>
+      <c r="D51" s="28"/>
+      <c r="E51" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="AL51" s="7"/>
+      <c r="AM51" s="7"/>
+      <c r="AN51" s="7"/>
+      <c r="AO51" s="7"/>
+      <c r="AP51" s="7"/>
+      <c r="AQ51" s="7"/>
+      <c r="AS51" s="7"/>
+      <c r="AU51" s="7"/>
+      <c r="AW51" s="7"/>
+      <c r="AY51" s="7"/>
       <c r="BD51" s="7"/>
       <c r="BI51" s="7"/>
     </row>
-    <row r="52" spans="2:61" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:61" x14ac:dyDescent="0.2">
       <c r="E52" s="1" t="s">
-        <v>22</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="AL52" s="7"/>
+      <c r="AM52" s="7"/>
+      <c r="AN52" s="7"/>
+      <c r="AO52" s="7"/>
+      <c r="AP52" s="7"/>
+      <c r="AQ52" s="7"/>
+      <c r="AS52" s="7"/>
+      <c r="AU52" s="7"/>
+      <c r="AW52" s="7"/>
+      <c r="AY52" s="7"/>
       <c r="BD52" s="7"/>
       <c r="BI52" s="7"/>
     </row>
-    <row r="53" spans="2:61" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:61" x14ac:dyDescent="0.2">
       <c r="E53" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="BD53" s="7"/>
       <c r="BI53" s="7"/>
     </row>
-    <row r="54" spans="2:61" x14ac:dyDescent="0.2">
-      <c r="E54" s="17" t="s">
-        <v>24</v>
+    <row r="54" spans="1:61" x14ac:dyDescent="0.2">
+      <c r="E54" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="BD54" s="7"/>
       <c r="BI54" s="7"/>
     </row>
-    <row r="55" spans="2:61" x14ac:dyDescent="0.2">
-      <c r="E55" s="22" t="s">
-        <v>27</v>
+    <row r="55" spans="1:61" x14ac:dyDescent="0.2">
+      <c r="E55" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="BD55" s="7"/>
       <c r="BI55" s="7"/>
     </row>
-    <row r="56" spans="2:61" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:61" x14ac:dyDescent="0.2">
+      <c r="E56" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="BD56" s="7"/>
       <c r="BI56" s="7"/>
     </row>
-    <row r="57" spans="2:61" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:61" x14ac:dyDescent="0.2">
+      <c r="E57" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="BD57" s="7"/>
       <c r="BI57" s="7"/>
     </row>
-    <row r="58" spans="2:61" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:61" x14ac:dyDescent="0.2">
+      <c r="E58" s="17" t="s">
+        <v>24</v>
+      </c>
       <c r="BD58" s="7"/>
       <c r="BI58" s="7"/>
     </row>
-    <row r="59" spans="2:61" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:61" x14ac:dyDescent="0.2">
+      <c r="E59" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="BD59" s="7"/>
       <c r="BI59" s="7"/>
     </row>
-    <row r="60" spans="2:61" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:61" x14ac:dyDescent="0.2">
       <c r="BD60" s="7"/>
       <c r="BI60" s="7"/>
     </row>
-    <row r="61" spans="2:61" x14ac:dyDescent="0.2">
-      <c r="B61" s="2"/>
-      <c r="C61" s="2"/>
-      <c r="D61" s="2"/>
-      <c r="E61" s="2"/>
-      <c r="F61" s="2"/>
-      <c r="G61" s="2"/>
-      <c r="H61" s="2"/>
-      <c r="I61" s="2"/>
-      <c r="J61" s="2"/>
-      <c r="K61" s="2"/>
-      <c r="L61" s="2"/>
-      <c r="M61" s="18"/>
-      <c r="N61" s="2"/>
-      <c r="O61" s="2"/>
-      <c r="P61" s="2"/>
-      <c r="S61" s="3"/>
-      <c r="T61" s="3"/>
-      <c r="U61" s="3"/>
-      <c r="W61" s="3"/>
-      <c r="AI61" s="3"/>
-    </row>
-    <row r="62" spans="2:61" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:61" x14ac:dyDescent="0.2">
+      <c r="BD61" s="7"/>
+      <c r="BI61" s="7"/>
+    </row>
+    <row r="62" spans="1:61" x14ac:dyDescent="0.2">
       <c r="BD62" s="7"/>
       <c r="BI62" s="7"/>
     </row>
-    <row r="63" spans="2:61" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:61" x14ac:dyDescent="0.2">
       <c r="BD63" s="7"/>
       <c r="BI63" s="7"/>
     </row>
-    <row r="64" spans="2:61" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:61" x14ac:dyDescent="0.2">
       <c r="BD64" s="7"/>
       <c r="BI64" s="7"/>
     </row>
-    <row r="65" spans="56:61" x14ac:dyDescent="0.2">
-      <c r="BD65" s="7"/>
-      <c r="BI65" s="7"/>
-    </row>
-    <row r="66" spans="56:61" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:61" x14ac:dyDescent="0.2">
+      <c r="B65" s="2"/>
+      <c r="C65" s="2"/>
+      <c r="D65" s="2"/>
+      <c r="E65" s="2"/>
+      <c r="F65" s="2"/>
+      <c r="G65" s="2"/>
+      <c r="H65" s="2"/>
+      <c r="I65" s="2"/>
+      <c r="J65" s="2"/>
+      <c r="K65" s="2"/>
+      <c r="L65" s="2"/>
+      <c r="M65" s="18"/>
+      <c r="N65" s="2"/>
+      <c r="O65" s="2"/>
+      <c r="P65" s="2"/>
+      <c r="S65" s="3"/>
+      <c r="T65" s="3"/>
+      <c r="U65" s="3"/>
+      <c r="W65" s="3"/>
+      <c r="AI65" s="3"/>
+    </row>
+    <row r="66" spans="2:61" x14ac:dyDescent="0.2">
       <c r="BD66" s="7"/>
       <c r="BI66" s="7"/>
     </row>
-    <row r="67" spans="56:61" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:61" x14ac:dyDescent="0.2">
       <c r="BD67" s="7"/>
       <c r="BI67" s="7"/>
     </row>
-    <row r="68" spans="56:61" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:61" x14ac:dyDescent="0.2">
       <c r="BD68" s="7"/>
       <c r="BI68" s="7"/>
     </row>
-    <row r="69" spans="56:61" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:61" x14ac:dyDescent="0.2">
       <c r="BD69" s="7"/>
       <c r="BI69" s="7"/>
     </row>
-    <row r="70" spans="56:61" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:61" x14ac:dyDescent="0.2">
       <c r="BD70" s="7"/>
       <c r="BI70" s="7"/>
     </row>
-    <row r="71" spans="56:61" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:61" x14ac:dyDescent="0.2">
       <c r="BD71" s="7"/>
       <c r="BI71" s="7"/>
     </row>
-    <row r="72" spans="56:61" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:61" x14ac:dyDescent="0.2">
       <c r="BD72" s="7"/>
       <c r="BI72" s="7"/>
     </row>
-    <row r="73" spans="56:61" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:61" x14ac:dyDescent="0.2">
       <c r="BD73" s="7"/>
       <c r="BI73" s="7"/>
     </row>
-    <row r="74" spans="56:61" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:61" x14ac:dyDescent="0.2">
       <c r="BD74" s="7"/>
       <c r="BI74" s="7"/>
     </row>
-    <row r="75" spans="56:61" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:61" x14ac:dyDescent="0.2">
       <c r="BD75" s="7"/>
       <c r="BI75" s="7"/>
     </row>
-    <row r="76" spans="56:61" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:61" x14ac:dyDescent="0.2">
       <c r="BD76" s="7"/>
       <c r="BI76" s="7"/>
     </row>
-    <row r="77" spans="56:61" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:61" x14ac:dyDescent="0.2">
       <c r="BD77" s="7"/>
       <c r="BI77" s="7"/>
     </row>
-    <row r="78" spans="56:61" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:61" x14ac:dyDescent="0.2">
       <c r="BD78" s="7"/>
       <c r="BI78" s="7"/>
     </row>
-    <row r="79" spans="56:61" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:61" x14ac:dyDescent="0.2">
       <c r="BD79" s="7"/>
       <c r="BI79" s="7"/>
     </row>
-    <row r="80" spans="56:61" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:61" x14ac:dyDescent="0.2">
       <c r="BD80" s="7"/>
       <c r="BI80" s="7"/>
     </row>
@@ -4482,15 +4779,19 @@
     </row>
     <row r="166" spans="56:61" x14ac:dyDescent="0.2">
       <c r="BD166" s="7"/>
+      <c r="BI166" s="7"/>
     </row>
     <row r="167" spans="56:61" x14ac:dyDescent="0.2">
       <c r="BD167" s="7"/>
+      <c r="BI167" s="7"/>
     </row>
     <row r="168" spans="56:61" x14ac:dyDescent="0.2">
       <c r="BD168" s="7"/>
+      <c r="BI168" s="7"/>
     </row>
     <row r="169" spans="56:61" x14ac:dyDescent="0.2">
       <c r="BD169" s="7"/>
+      <c r="BI169" s="7"/>
     </row>
     <row r="170" spans="56:61" x14ac:dyDescent="0.2">
       <c r="BD170" s="7"/>
@@ -4542,6 +4843,18 @@
     </row>
     <row r="186" spans="56:56" x14ac:dyDescent="0.2">
       <c r="BD186" s="7"/>
+    </row>
+    <row r="187" spans="56:56" x14ac:dyDescent="0.2">
+      <c r="BD187" s="7"/>
+    </row>
+    <row r="188" spans="56:56" x14ac:dyDescent="0.2">
+      <c r="BD188" s="7"/>
+    </row>
+    <row r="189" spans="56:56" x14ac:dyDescent="0.2">
+      <c r="BD189" s="7"/>
+    </row>
+    <row r="190" spans="56:56" x14ac:dyDescent="0.2">
+      <c r="BD190" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>